<commit_message>
check here for the oldest filter
</commit_message>
<xml_diff>
--- a/tests/test_data/gen_puck_table/GOOD_sample_boltz_bxyl.xlsx
+++ b/tests/test_data/gen_puck_table/GOOD_sample_boltz_bxyl.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-19200" yWindow="-24000" windowWidth="19200" windowHeight="23560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="20400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="z_cluster-sorted-ALL-bxyl-am1.c" sheetId="1" r:id="rId1"/>
@@ -709,7 +709,7 @@
   <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -858,7 +858,7 @@
         <v>2.6518211310827457E-3</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O23" si="4">SUMIF($G$2:$G$33,$M3,$K$2:$K$33)</f>
+        <f>SUMIF($G$2:$G$33,$M3,$K$2:$K$33)</f>
         <v>3.96722728365273</v>
       </c>
     </row>
@@ -893,7 +893,7 @@
         <v>1.2602245746474051E-6</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" ref="J3:J33" si="5">I4/INDEX($N$2:$N$23,MATCH($G4,$M$2:$M$23,0))</f>
+        <f t="shared" ref="J4:J33" si="4">I4/INDEX($N$2:$N$23,MATCH($G4,$M$2:$M$23,0))</f>
         <v>1.2776239486226418E-4</v>
       </c>
       <c r="K4" s="1">
@@ -908,7 +908,7 @@
         <v>9.8638145911870683E-3</v>
       </c>
       <c r="O4">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="O3:O23" si="5">SUMIF($G$2:$G$33,$M4,$K$2:$K$33)</f>
         <v>2.9858006124067162</v>
       </c>
     </row>
@@ -943,7 +943,7 @@
         <v>1.4939310127274929E-3</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.15145570701037525</v>
       </c>
       <c r="K5" s="1">
@@ -958,7 +958,7 @@
         <v>8.9309493990124746E-3</v>
       </c>
       <c r="O5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.8435787778844221</v>
       </c>
     </row>
@@ -993,7 +993,7 @@
         <v>1.2995215416655216E-4</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.9004871649654717E-2</v>
       </c>
       <c r="K6" s="1">
@@ -1008,7 +1008,7 @@
         <v>3.8667236185990065E-5</v>
       </c>
       <c r="O6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.3974409951064963</v>
       </c>
     </row>
@@ -1043,7 +1043,7 @@
         <v>1.5332837642922914E-4</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.7168205705675947E-2</v>
       </c>
       <c r="K7" s="1">
@@ -1058,7 +1058,7 @@
         <v>1.059561949876211E-3</v>
       </c>
       <c r="O7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.0537113699999789</v>
       </c>
     </row>
@@ -1093,7 +1093,7 @@
         <v>1.3681308605366139E-5</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.35382173526855687</v>
       </c>
       <c r="K8" s="1">
@@ -1108,7 +1108,7 @@
         <v>1.8005238943154784E-5</v>
       </c>
       <c r="O8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.4652303784999692</v>
       </c>
     </row>
@@ -1143,7 +1143,7 @@
         <v>1.059561949876211E-3</v>
       </c>
       <c r="J9" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K9" s="1">
@@ -1158,7 +1158,7 @@
         <v>7.9876533022209403E-4</v>
       </c>
       <c r="O9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.257049727249604</v>
       </c>
     </row>
@@ -1193,7 +1193,7 @@
         <v>1.8005238943154784E-5</v>
       </c>
       <c r="J10" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K10" s="1">
@@ -1208,7 +1208,7 @@
         <v>1.2764750851623598E-4</v>
       </c>
       <c r="O10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.354468890092674</v>
       </c>
     </row>
@@ -1243,7 +1243,7 @@
         <v>3.6384497920872366E-2</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.9919670409117114</v>
       </c>
       <c r="K11" s="1">
@@ -1258,7 +1258,7 @@
         <v>0.38673694643236034</v>
       </c>
       <c r="O11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.642663342900058</v>
       </c>
     </row>
@@ -1293,7 +1293,7 @@
         <v>8.8764821212361641E-6</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.1112753377475819E-2</v>
       </c>
       <c r="K12" s="1">
@@ -1308,7 +1308,7 @@
         <v>3.7087252840125988E-4</v>
       </c>
       <c r="O12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.6749457749999728</v>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
         <v>8.3686233538849287E-3</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.84841653059476252</v>
       </c>
       <c r="K13" s="1">
@@ -1358,7 +1358,7 @@
         <v>1.9320261927431869E-4</v>
       </c>
       <c r="O13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.0608641174999933</v>
       </c>
     </row>
@@ -1393,7 +1393,7 @@
         <v>1.7814542126614113E-3</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.67178520895715121</v>
       </c>
       <c r="K14" s="1">
@@ -1408,7 +1408,7 @@
         <v>1.5695416426238976E-6</v>
       </c>
       <c r="O14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.9091297380000025</v>
       </c>
     </row>
@@ -1443,7 +1443,7 @@
         <v>8.7776210225832454E-3</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.98283179429432399</v>
       </c>
       <c r="K15" s="1">
@@ -1458,7 +1458,7 @@
         <v>1.7468872218381586E-4</v>
       </c>
       <c r="O15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.1204775200000006</v>
       </c>
     </row>
@@ -1493,7 +1493,7 @@
         <v>2.0308412894912197E-6</v>
       </c>
       <c r="J16" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.5909760504513953E-2</v>
       </c>
       <c r="K16" s="1">
@@ -1508,7 +1508,7 @@
         <v>6.6915297115779891E-7</v>
       </c>
       <c r="O16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.4136473759999841</v>
       </c>
     </row>
@@ -1543,7 +1543,7 @@
         <v>1.2561666722674475E-4</v>
       </c>
       <c r="J17" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.98409023949548602</v>
       </c>
       <c r="K17" s="1">
@@ -1558,7 +1558,7 @@
         <v>2.2795654389260158E-4</v>
       </c>
       <c r="O17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.9629726354999999</v>
       </c>
     </row>
@@ -1593,7 +1593,7 @@
         <v>0.37499998500485859</v>
       </c>
       <c r="J18" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.96965130553008971</v>
       </c>
       <c r="K18" s="1">
@@ -1608,7 +1608,7 @@
         <v>6.0405562117320972E-6</v>
       </c>
       <c r="O18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.1115651634999884</v>
       </c>
     </row>
@@ -1643,7 +1643,7 @@
         <v>3.7087252840125988E-4</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K19" s="1">
@@ -1658,7 +1658,7 @@
         <v>1.2059445391540046E-5</v>
       </c>
       <c r="O19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.7024289694999979</v>
       </c>
     </row>
@@ -1693,7 +1693,7 @@
         <v>1.1736961427501724E-2</v>
       </c>
       <c r="J20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.0348694469910179E-2</v>
       </c>
       <c r="K20" s="1">
@@ -1708,7 +1708,7 @@
         <v>9.2070136539715099E-5</v>
       </c>
       <c r="O20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.4994932579999967</v>
       </c>
     </row>
@@ -1743,7 +1743,7 @@
         <v>1.9320261927431869E-4</v>
       </c>
       <c r="J21" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K21" s="1">
@@ -1758,7 +1758,7 @@
         <v>1.1173027013965598E-5</v>
       </c>
       <c r="O21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.747609653499973</v>
       </c>
     </row>
@@ -1793,7 +1793,7 @@
         <v>1.5695416426238976E-6</v>
       </c>
       <c r="J22" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K22" s="1">
@@ -1808,7 +1808,7 @@
         <v>1.1309856586797966E-4</v>
       </c>
       <c r="O22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.377756414999979</v>
       </c>
     </row>
@@ -1843,7 +1843,7 @@
         <v>1.7468872218381586E-4</v>
       </c>
       <c r="J23" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K23" s="1">
@@ -1858,7 +1858,7 @@
         <v>5.6231950175295254E-5</v>
       </c>
       <c r="O23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.7912851754999917</v>
       </c>
     </row>
@@ -1893,7 +1893,7 @@
         <v>6.6915297115779891E-7</v>
       </c>
       <c r="J24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K24" s="1">
@@ -1932,7 +1932,7 @@
         <v>2.2795654389260158E-4</v>
       </c>
       <c r="J25" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K25" s="1">
@@ -1971,7 +1971,7 @@
         <v>6.0405562117320972E-6</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K26" s="1">
@@ -2010,7 +2010,7 @@
         <v>1.2059445391540046E-5</v>
       </c>
       <c r="J27" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K27" s="1">
@@ -2049,7 +2049,7 @@
         <v>9.2070136539715099E-5</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K28" s="1">
@@ -2088,7 +2088,7 @@
         <v>1.1173027013965598E-5</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K29" s="1">
@@ -2127,7 +2127,7 @@
         <v>1.1309856586797966E-4</v>
       </c>
       <c r="J30" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K30" s="1">
@@ -2166,7 +2166,7 @@
         <v>5.6231950175295254E-5</v>
       </c>
       <c r="J31" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K31" s="1">
@@ -2205,7 +2205,7 @@
         <v>7.8988884810085786E-4</v>
       </c>
       <c r="J32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.98888724662252414</v>
       </c>
       <c r="K32" s="1">
@@ -2244,7 +2244,7 @@
         <v>2.4985927580623929E-5</v>
       </c>
       <c r="J33" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.64617826473144324</v>
       </c>
       <c r="K33" s="1">

</xml_diff>